<commit_message>
atualizaçao: add parte que executa o .ps1, em fase de teste
</commit_message>
<xml_diff>
--- a/dados_planilha.xlsx
+++ b/dados_planilha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7b7fab9242a38aa1/Anexos/Área de Trabalho/projeto_users/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="14_{41638726-F171-4776-80CA-9962D6C11B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B94EAD4D-228E-4AAC-99D6-14CCD0446771}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="14_{41638726-F171-4776-80CA-9962D6C11B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43BF7E9B-96DF-4FD1-928E-093419CAD427}"/>
   <bookViews>
     <workbookView xWindow="5760" yWindow="696" windowWidth="17280" windowHeight="8880" xr2:uid="{02D1EADD-FA41-4C5D-B9D2-551FFF10C9F6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="9">
   <si>
     <t>CPF</t>
   </si>
@@ -218,7 +218,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -227,9 +227,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -239,9 +236,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -267,9 +261,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -288,11 +279,11 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -637,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23EEC73F-E6DE-4DE3-A743-FAC743BD83DD}">
   <dimension ref="B1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -652,14 +643,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -682,323 +673,503 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="23">
-        <v>595619</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="15"/>
-    </row>
-    <row r="4" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="24"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="17"/>
-    </row>
-    <row r="5" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="17"/>
-    </row>
-    <row r="6" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="17"/>
-    </row>
-    <row r="7" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="17"/>
-    </row>
-    <row r="8" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="17"/>
-    </row>
-    <row r="9" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="17"/>
-    </row>
-    <row r="10" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="17"/>
-    </row>
-    <row r="11" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="17"/>
-    </row>
-    <row r="12" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="17"/>
-    </row>
-    <row r="13" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="17"/>
-    </row>
-    <row r="14" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="17"/>
-    </row>
-    <row r="15" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="17"/>
-    </row>
-    <row r="16" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="17"/>
-    </row>
-    <row r="17" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="17"/>
-    </row>
-    <row r="18" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="17"/>
-    </row>
-    <row r="19" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="17"/>
-    </row>
-    <row r="20" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="17"/>
-    </row>
-    <row r="21" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="17"/>
-    </row>
-    <row r="22" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="17"/>
-    </row>
-    <row r="23" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="17"/>
-    </row>
-    <row r="24" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="17"/>
-    </row>
-    <row r="25" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="17"/>
-    </row>
-    <row r="26" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="17"/>
-    </row>
-    <row r="27" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="17"/>
-    </row>
-    <row r="28" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="17"/>
-    </row>
-    <row r="29" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="17"/>
-    </row>
-    <row r="30" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="17"/>
-    </row>
-    <row r="31" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="17"/>
-    </row>
-    <row r="32" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="17"/>
+    <row r="3" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="13"/>
+    </row>
+    <row r="4" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="13"/>
+    </row>
+    <row r="6" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="13"/>
+    </row>
+    <row r="7" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="13"/>
+    </row>
+    <row r="8" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="11"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="13"/>
+    </row>
+    <row r="10" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="11"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="13"/>
+    </row>
+    <row r="11" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="13"/>
+    </row>
+    <row r="12" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="13"/>
+    </row>
+    <row r="14" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="13"/>
+    </row>
+    <row r="16" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="11"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="19" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="11"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="13"/>
+    </row>
+    <row r="20" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="11"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="13"/>
+    </row>
+    <row r="21" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="13"/>
+    </row>
+    <row r="22" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="13"/>
+    </row>
+    <row r="23" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="13"/>
+    </row>
+    <row r="24" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="13"/>
+    </row>
+    <row r="25" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="11"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="13"/>
+    </row>
+    <row r="26" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="11"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="13"/>
+    </row>
+    <row r="27" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="11"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="13"/>
+    </row>
+    <row r="28" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="11"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="13"/>
+    </row>
+    <row r="29" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="11"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="13"/>
+    </row>
+    <row r="30" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="11"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="13"/>
+    </row>
+    <row r="31" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="11"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="13"/>
+    </row>
+    <row r="32" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="11"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="17"/>
+      <c r="B33" s="20">
+        <v>595619</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="11"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="17"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="15"/>
     </row>
     <row r="35" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="17"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="15"/>
     </row>
     <row r="36" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="17"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="15"/>
     </row>
     <row r="37" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="17"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="15"/>
     </row>
     <row r="38" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="17"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="15"/>
     </row>
     <row r="39" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="17"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="15"/>
     </row>
     <row r="40" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="20"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="17"/>
     </row>
     <row r="41" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="22"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>